<commit_message>
added Scatter Plot: doc/Examples/src-plot/Scatter.js
</commit_message>
<xml_diff>
--- a/data/Book1.xlsx
+++ b/data/Book1.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\JS-SVG-Client\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6C5068-A364-4EB8-98D0-2800891ED9BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D7E92C-D875-45E6-B6B9-E8F1D549FEEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{ACF4154E-FD6B-4497-B4DB-14320FF8EFDB}"/>
+    <workbookView xWindow="13710" yWindow="1605" windowWidth="15090" windowHeight="13875" activeTab="2" xr2:uid="{ACF4154E-FD6B-4497-B4DB-14320FF8EFDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="sport" sheetId="2" r:id="rId2"/>
-    <sheet name="population" sheetId="6" r:id="rId3"/>
-    <sheet name="expenses" sheetId="3" r:id="rId4"/>
-    <sheet name="sales" sheetId="4" r:id="rId5"/>
-    <sheet name="temperature" sheetId="5" r:id="rId6"/>
+    <sheet name="Anscombe" sheetId="7" r:id="rId3"/>
+    <sheet name="population" sheetId="6" r:id="rId4"/>
+    <sheet name="expenses" sheetId="3" r:id="rId5"/>
+    <sheet name="sales" sheetId="4" r:id="rId6"/>
+    <sheet name="temperature" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="83">
   <si>
     <t>x</t>
   </si>
@@ -264,6 +265,21 @@
   </si>
   <si>
     <t>Disability</t>
+  </si>
+  <si>
+    <t>Dataset I</t>
+  </si>
+  <si>
+    <t>Dataset II</t>
+  </si>
+  <si>
+    <t>Dataset III</t>
+  </si>
+  <si>
+    <t>Dataset IV</t>
+  </si>
+  <si>
+    <t>Anscombe's quartet</t>
   </si>
 </sst>
 </file>
@@ -271,9 +287,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -291,6 +307,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -316,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -333,7 +357,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1072,6 +1111,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-450E-44ED-B9F2-D85B1CA0CB36}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1087,6 +1131,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-450E-44ED-B9F2-D85B1CA0CB36}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1102,6 +1151,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-450E-44ED-B9F2-D85B1CA0CB36}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -1117,6 +1171,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-450E-44ED-B9F2-D85B1CA0CB36}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -1132,6 +1191,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-450E-44ED-B9F2-D85B1CA0CB36}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -1147,6 +1211,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-450E-44ED-B9F2-D85B1CA0CB36}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -3605,7 +3674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DC727EE-B0FC-4C7D-961C-CC5730B4F1FA}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="280" zoomScaleNormal="280" workbookViewId="0">
+    <sheetView zoomScale="280" zoomScaleNormal="280" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -3738,6 +3807,404 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2786D27-6ADC-45C0-B36F-885854621D2D}">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="H2" s="8"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>10</v>
+      </c>
+      <c r="B4" s="7">
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="C4" s="7">
+        <v>10</v>
+      </c>
+      <c r="D4" s="7">
+        <v>9.14</v>
+      </c>
+      <c r="E4" s="7">
+        <v>10</v>
+      </c>
+      <c r="F4" s="7">
+        <v>7.46</v>
+      </c>
+      <c r="G4" s="7">
+        <v>8</v>
+      </c>
+      <c r="H4" s="7">
+        <v>6.58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>8</v>
+      </c>
+      <c r="B5" s="7">
+        <v>6.95</v>
+      </c>
+      <c r="C5" s="7">
+        <v>8</v>
+      </c>
+      <c r="D5" s="7">
+        <v>8.14</v>
+      </c>
+      <c r="E5" s="7">
+        <v>8</v>
+      </c>
+      <c r="F5" s="7">
+        <v>6.77</v>
+      </c>
+      <c r="G5" s="7">
+        <v>8</v>
+      </c>
+      <c r="H5" s="7">
+        <v>5.76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>13</v>
+      </c>
+      <c r="B6" s="7">
+        <v>7.58</v>
+      </c>
+      <c r="C6" s="7">
+        <v>13</v>
+      </c>
+      <c r="D6" s="7">
+        <v>8.74</v>
+      </c>
+      <c r="E6" s="7">
+        <v>13</v>
+      </c>
+      <c r="F6" s="7">
+        <v>12.74</v>
+      </c>
+      <c r="G6" s="7">
+        <v>8</v>
+      </c>
+      <c r="H6" s="7">
+        <v>7.71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>9</v>
+      </c>
+      <c r="B7" s="7">
+        <v>8.81</v>
+      </c>
+      <c r="C7" s="7">
+        <v>9</v>
+      </c>
+      <c r="D7" s="7">
+        <v>8.77</v>
+      </c>
+      <c r="E7" s="7">
+        <v>9</v>
+      </c>
+      <c r="F7" s="7">
+        <v>7.11</v>
+      </c>
+      <c r="G7" s="7">
+        <v>8</v>
+      </c>
+      <c r="H7" s="7">
+        <v>8.84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>11</v>
+      </c>
+      <c r="B8" s="7">
+        <v>8.33</v>
+      </c>
+      <c r="C8" s="7">
+        <v>11</v>
+      </c>
+      <c r="D8" s="7">
+        <v>9.26</v>
+      </c>
+      <c r="E8" s="7">
+        <v>11</v>
+      </c>
+      <c r="F8" s="7">
+        <v>7.81</v>
+      </c>
+      <c r="G8" s="7">
+        <v>8</v>
+      </c>
+      <c r="H8" s="7">
+        <v>8.4700000000000006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>14</v>
+      </c>
+      <c r="B9" s="7">
+        <v>9.9600000000000009</v>
+      </c>
+      <c r="C9" s="7">
+        <v>14</v>
+      </c>
+      <c r="D9" s="7">
+        <v>8.1</v>
+      </c>
+      <c r="E9" s="7">
+        <v>14</v>
+      </c>
+      <c r="F9" s="7">
+        <v>8.84</v>
+      </c>
+      <c r="G9" s="7">
+        <v>8</v>
+      </c>
+      <c r="H9" s="7">
+        <v>7.04</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>6</v>
+      </c>
+      <c r="B10" s="7">
+        <v>7.24</v>
+      </c>
+      <c r="C10" s="7">
+        <v>6</v>
+      </c>
+      <c r="D10" s="7">
+        <v>6.13</v>
+      </c>
+      <c r="E10" s="7">
+        <v>6</v>
+      </c>
+      <c r="F10" s="7">
+        <v>6.08</v>
+      </c>
+      <c r="G10" s="7">
+        <v>8</v>
+      </c>
+      <c r="H10" s="7">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>4</v>
+      </c>
+      <c r="B11" s="7">
+        <v>4.26</v>
+      </c>
+      <c r="C11" s="7">
+        <v>4</v>
+      </c>
+      <c r="D11" s="7">
+        <v>3.1</v>
+      </c>
+      <c r="E11" s="7">
+        <v>4</v>
+      </c>
+      <c r="F11" s="7">
+        <v>5.39</v>
+      </c>
+      <c r="G11" s="7">
+        <v>19</v>
+      </c>
+      <c r="H11" s="7">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>12</v>
+      </c>
+      <c r="B12" s="7">
+        <v>10.84</v>
+      </c>
+      <c r="C12" s="7">
+        <v>12</v>
+      </c>
+      <c r="D12" s="7">
+        <v>9.1300000000000008</v>
+      </c>
+      <c r="E12" s="7">
+        <v>12</v>
+      </c>
+      <c r="F12" s="7">
+        <v>8.15</v>
+      </c>
+      <c r="G12" s="7">
+        <v>8</v>
+      </c>
+      <c r="H12" s="7">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>7</v>
+      </c>
+      <c r="B13" s="7">
+        <v>4.82</v>
+      </c>
+      <c r="C13" s="7">
+        <v>7</v>
+      </c>
+      <c r="D13" s="7">
+        <v>7.26</v>
+      </c>
+      <c r="E13" s="7">
+        <v>7</v>
+      </c>
+      <c r="F13" s="7">
+        <v>6.42</v>
+      </c>
+      <c r="G13" s="7">
+        <v>8</v>
+      </c>
+      <c r="H13" s="7">
+        <v>7.91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>5</v>
+      </c>
+      <c r="B14" s="7">
+        <v>5.68</v>
+      </c>
+      <c r="C14" s="7">
+        <v>5</v>
+      </c>
+      <c r="D14" s="7">
+        <v>4.74</v>
+      </c>
+      <c r="E14" s="7">
+        <v>5</v>
+      </c>
+      <c r="F14" s="7">
+        <v>5.73</v>
+      </c>
+      <c r="G14" s="7">
+        <v>8</v>
+      </c>
+      <c r="H14" s="7">
+        <v>6.89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <f>MIN(A4:A14)</f>
+        <v>4</v>
+      </c>
+      <c r="B15" s="10">
+        <f>MIN(B4:B14)</f>
+        <v>4.26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <f>MAX(A4:A14)</f>
+        <v>14</v>
+      </c>
+      <c r="B16" s="10">
+        <f>MAX(B4:B14)</f>
+        <v>10.84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <f>SUM(A4:A14)</f>
+        <v>99</v>
+      </c>
+      <c r="B17" s="10">
+        <f>SUM(B4:B14)</f>
+        <v>82.510000000000019</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C826C821-FF9A-44ED-9BA5-C55A680AF63A}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -3823,7 +4290,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78AB892E-AC5C-4475-B05C-C05CBC73E516}">
   <dimension ref="A1:M12"/>
   <sheetViews>
@@ -4085,7 +4552,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A732BD7-EA3E-419B-8AC9-7C03E7AB2404}">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -4227,7 +4694,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8D6F23-EA4E-47B3-A513-3DBE6F5374D7}">
   <dimension ref="A1:D13"/>
   <sheetViews>

</xml_diff>

<commit_message>
added Bubble Chart: doc/Examples/src-plot/Bubble.js
</commit_message>
<xml_diff>
--- a/data/Book1.xlsx
+++ b/data/Book1.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\JS-SVG-Client\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D7E92C-D875-45E6-B6B9-E8F1D549FEEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72BBEE2-BFE3-4DCC-BA80-6E8C3048D610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13710" yWindow="1605" windowWidth="15090" windowHeight="13875" activeTab="2" xr2:uid="{ACF4154E-FD6B-4497-B4DB-14320FF8EFDB}"/>
+    <workbookView xWindow="13710" yWindow="1605" windowWidth="15090" windowHeight="13875" activeTab="3" xr2:uid="{ACF4154E-FD6B-4497-B4DB-14320FF8EFDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="sport" sheetId="2" r:id="rId2"/>
     <sheet name="Anscombe" sheetId="7" r:id="rId3"/>
-    <sheet name="population" sheetId="6" r:id="rId4"/>
-    <sheet name="expenses" sheetId="3" r:id="rId5"/>
-    <sheet name="sales" sheetId="4" r:id="rId6"/>
-    <sheet name="temperature" sheetId="5" r:id="rId7"/>
+    <sheet name="Bubble" sheetId="8" r:id="rId4"/>
+    <sheet name="population" sheetId="6" r:id="rId5"/>
+    <sheet name="expenses" sheetId="3" r:id="rId6"/>
+    <sheet name="sales" sheetId="4" r:id="rId7"/>
+    <sheet name="temperature" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="121">
   <si>
     <t>x</t>
   </si>
@@ -280,6 +281,120 @@
   </si>
   <si>
     <t>Anscombe's quartet</t>
+  </si>
+  <si>
+    <t>Sugar and fat intake per country</t>
+  </si>
+  <si>
+    <t>Daily fat intake</t>
+  </si>
+  <si>
+    <t>Series 1</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>NZ</t>
+  </si>
+  <si>
+    <t>HU</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>RU</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>ES</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>NL</t>
+  </si>
+  <si>
+    <t>FI</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>New Zealand</t>
+  </si>
+  <si>
+    <t>Hungary</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Alpha2</t>
+  </si>
+  <si>
+    <t>x=fat</t>
+  </si>
+  <si>
+    <t>y=sugar</t>
+  </si>
+  <si>
+    <t>z=obesity</t>
   </si>
 </sst>
 </file>
@@ -340,7 +455,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -370,8 +485,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3810,7 +3942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2786D27-6ADC-45C0-B36F-885854621D2D}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -3820,34 +3952,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="11"/>
+      <c r="C2" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8" t="s">
+      <c r="D2" s="11"/>
+      <c r="E2" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8" t="s">
+      <c r="F2" s="11"/>
+      <c r="G2" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="H2" s="8"/>
+      <c r="H2" s="11"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
@@ -4205,6 +4337,400 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{942E0003-48E9-49DF-99D5-B3E52D4AC7F6}">
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="15.42578125" style="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
+      <c r="B3" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="17">
+        <v>63.4</v>
+      </c>
+      <c r="C4" s="17">
+        <v>51.8</v>
+      </c>
+      <c r="D4" s="18">
+        <v>15.4</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="17">
+        <v>64</v>
+      </c>
+      <c r="C5" s="17">
+        <v>82.9</v>
+      </c>
+      <c r="D5" s="18">
+        <v>31.3</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="17">
+        <v>65.400000000000006</v>
+      </c>
+      <c r="C6" s="17">
+        <v>50.8</v>
+      </c>
+      <c r="D6" s="18">
+        <v>28.5</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="17">
+        <v>65.5</v>
+      </c>
+      <c r="C7" s="17">
+        <v>126.4</v>
+      </c>
+      <c r="D7" s="18">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="17">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="C8" s="17">
+        <v>20</v>
+      </c>
+      <c r="D8" s="18">
+        <v>16</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="17">
+        <v>69.2</v>
+      </c>
+      <c r="C9" s="17">
+        <v>57.6</v>
+      </c>
+      <c r="D9" s="18">
+        <v>10.4</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" s="17">
+        <v>71</v>
+      </c>
+      <c r="C10" s="17">
+        <v>93.2</v>
+      </c>
+      <c r="D10" s="18">
+        <v>24.7</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="17">
+        <v>73.5</v>
+      </c>
+      <c r="C11" s="17">
+        <v>83.1</v>
+      </c>
+      <c r="D11" s="18">
+        <v>10</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" s="17">
+        <v>74.2</v>
+      </c>
+      <c r="C12" s="17">
+        <v>68.5</v>
+      </c>
+      <c r="D12" s="18">
+        <v>14.5</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13" s="17">
+        <v>78.400000000000006</v>
+      </c>
+      <c r="C13" s="17">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="D13" s="18">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="17">
+        <v>80.3</v>
+      </c>
+      <c r="C14" s="17">
+        <v>86.1</v>
+      </c>
+      <c r="D14" s="18">
+        <v>11.8</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="17">
+        <v>80.400000000000006</v>
+      </c>
+      <c r="C15" s="17">
+        <v>102.5</v>
+      </c>
+      <c r="D15" s="18">
+        <v>12</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16" s="17">
+        <v>80.8</v>
+      </c>
+      <c r="C16" s="17">
+        <v>91.5</v>
+      </c>
+      <c r="D16" s="18">
+        <v>15.8</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17" s="17">
+        <v>86.5</v>
+      </c>
+      <c r="C17" s="17">
+        <v>102.9</v>
+      </c>
+      <c r="D17" s="18">
+        <v>14.7</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B18" s="17">
+        <v>95</v>
+      </c>
+      <c r="C18" s="17">
+        <v>95</v>
+      </c>
+      <c r="D18" s="18">
+        <v>13.8</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="6">
+        <f>MIN(B4:B18)</f>
+        <v>63.4</v>
+      </c>
+      <c r="C19" s="6">
+        <f>MIN(C4:C18)</f>
+        <v>20</v>
+      </c>
+      <c r="D19" s="6">
+        <f>MIN(D4:D18)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="6">
+        <f>MAX(B5:B19)</f>
+        <v>95</v>
+      </c>
+      <c r="C20" s="6">
+        <f>MAX(C5:C19)</f>
+        <v>126.4</v>
+      </c>
+      <c r="D20" s="6">
+        <f>MAX(D5:D19)</f>
+        <v>35.299999999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C826C821-FF9A-44ED-9BA5-C55A680AF63A}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -4290,7 +4816,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78AB892E-AC5C-4475-B05C-C05CBC73E516}">
   <dimension ref="A1:M12"/>
   <sheetViews>
@@ -4552,7 +5078,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A732BD7-EA3E-419B-8AC9-7C03E7AB2404}">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -4694,7 +5220,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8D6F23-EA4E-47B3-A513-3DBE6F5374D7}">
   <dimension ref="A1:D13"/>
   <sheetViews>

</xml_diff>